<commit_message>
destination upload and download done
</commit_message>
<xml_diff>
--- a/uploads/Learning_Destination.xlsx
+++ b/uploads/Learning_Destination.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lincoln Uni\Computing\639\pj2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4515144-E00B-46E5-8FD8-AE8191609DEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0692FE-061E-4840-9240-E3B6E6638637}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0206F248-0706-4A9D-9D3A-F1C1380B0ADD}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="59">
   <si>
     <t>#</t>
   </si>
@@ -143,9 +143,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.ccc.govt.nz/ </t>
-  </si>
-  <si>
-    <t>Free</t>
   </si>
   <si>
     <t>Pending</t>
@@ -675,8 +672,8 @@
   </sheetPr>
   <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -756,7 +753,7 @@
         <v>20</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>18</v>
@@ -863,11 +860,11 @@
       <c r="K3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>36</v>
+      <c r="L3" s="9">
+        <v>0</v>
+      </c>
+      <c r="M3" s="9">
+        <v>0</v>
       </c>
       <c r="N3" s="6">
         <v>43503</v>
@@ -900,23 +897,23 @@
         <v>29</v>
       </c>
       <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="E4" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="F4" s="11" t="s">
         <v>39</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>40</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>25</v>
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L4" s="5">
         <v>15</v>
@@ -934,7 +931,7 @@
         <v>29</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R4" s="7" t="s">
         <v>29</v>
@@ -947,7 +944,7 @@
         <v>30</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
@@ -964,7 +961,7 @@
     <hyperlink ref="K4" r:id="rId2" xr:uid="{927146F4-935B-4192-BDB1-9C8962EF4929}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" orientation="landscape"/>
+  <pageSetup paperSize="8" orientation="landscape" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -989,64 +986,64 @@
         <v>2</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="D1" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="E1" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
         <v>47</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>48</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>49</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>50</v>
-      </c>
-      <c r="E2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
         <v>52</v>
       </c>
-      <c r="B3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>53</v>
-      </c>
-      <c r="E3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
         <v>55</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
         <v>56</v>
       </c>
-      <c r="C4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>57</v>
-      </c>
-      <c r="E4" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1060,21 +1057,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100840061F9DC321B428F6D5C5DB03A1A63" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="218d44522063d3e139a84098689cd5f5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="180eb382-7469-4407-b6a7-9e3c553560d8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7bb75e2003902cea2fab401753615262" ns2:_="">
     <xsd:import namespace="180eb382-7469-4407-b6a7-9e3c553560d8"/>
@@ -1252,24 +1234,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8631EF32-6A38-459F-AD24-E2400611BAC5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4880AF2-56D8-434C-A4B7-226F046B614C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1ECE128-4AFA-4D9A-A791-7A9B74B8B681}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1285,4 +1265,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4880AF2-56D8-434C-A4B7-226F046B614C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8631EF32-6A38-459F-AD24-E2400611BAC5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
ld download upload done
</commit_message>
<xml_diff>
--- a/uploads/Learning_Destination.xlsx
+++ b/uploads/Learning_Destination.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lincoln Uni\Computing\639\pj2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0692FE-061E-4840-9240-E3B6E6638637}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B481FCE8-6496-43CF-9930-448A93300417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0206F248-0706-4A9D-9D3A-F1C1380B0ADD}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="58">
   <si>
     <t>#</t>
   </si>
@@ -91,12 +91,6 @@
     <t>Initial Fb Promo</t>
   </si>
   <si>
-    <t xml:space="preserve">2020 Paperwork </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021 Paperwork </t>
-  </si>
-  <si>
     <t>Photo provided</t>
   </si>
   <si>
@@ -212,6 +206,9 @@
   </si>
   <si>
     <t>Note</t>
+  </si>
+  <si>
+    <t>Paperwork</t>
   </si>
 </sst>
 </file>
@@ -313,7 +310,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -348,6 +345,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -670,10 +670,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V11"/>
+  <dimension ref="A1:AI12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="Z11" sqref="Z11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -694,271 +694,298 @@
     <col min="22" max="22" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="54.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:35" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="U1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" ht="54.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="U1" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="T2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U2" s="1">
+        <v>2020</v>
+      </c>
+      <c r="V2" s="1">
+        <v>2021</v>
+      </c>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A2" s="10">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
         <v>1</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="4">
-        <v>9.5</v>
-      </c>
-      <c r="M2" s="5">
-        <v>46</v>
-      </c>
-      <c r="N2" s="6">
-        <v>43501</v>
-      </c>
-      <c r="O2" s="6">
-        <v>43501</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A3" s="10">
-        <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="4">
+        <v>9.5</v>
+      </c>
+      <c r="M3" s="5">
+        <v>46</v>
+      </c>
+      <c r="N3" s="6">
+        <v>43501</v>
+      </c>
+      <c r="O3" s="6">
+        <v>43501</v>
+      </c>
+      <c r="P3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="Q3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="8"/>
-      <c r="K3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="9">
-        <v>0</v>
-      </c>
-      <c r="M3" s="9">
-        <v>0</v>
-      </c>
-      <c r="N3" s="6">
-        <v>43503</v>
-      </c>
-      <c r="O3" s="6">
-        <v>43503</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>29</v>
-      </c>
       <c r="R3" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="T3" s="2"/>
       <c r="U3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="V3" s="2"/>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
+        <v>2</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="V3" s="2" t="s">
-        <v>30</v>
+      <c r="F4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="8"/>
+      <c r="K4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="9">
+        <v>0</v>
+      </c>
+      <c r="M4" s="9">
+        <v>0</v>
+      </c>
+      <c r="N4" s="6">
+        <v>43503</v>
+      </c>
+      <c r="O4" s="6">
+        <v>43503</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:22" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10">
+    <row r="5" spans="1:35" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
         <v>29</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="F5" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="G5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="L5" s="5">
+        <v>15</v>
+      </c>
+      <c r="M5" s="5">
+        <v>15</v>
+      </c>
+      <c r="N5" s="6">
+        <v>43546</v>
+      </c>
+      <c r="O5" s="6">
+        <v>43181</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q5" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" s="5">
-        <v>15</v>
-      </c>
-      <c r="M4" s="5">
-        <v>15</v>
-      </c>
-      <c r="N4" s="6">
-        <v>43546</v>
-      </c>
-      <c r="O4" s="6">
-        <v>43181</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="R4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="S4" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="T4" s="13"/>
-      <c r="U4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>41</v>
+      <c r="R5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S5" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="T5" s="13"/>
+      <c r="U5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="U6" s="15"/>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" xr:uid="{066D7A64-2A15-493A-89F9-E21854D10CBE}"/>
-    <hyperlink ref="K4" r:id="rId2" xr:uid="{927146F4-935B-4192-BDB1-9C8962EF4929}"/>
+    <hyperlink ref="K3" r:id="rId1" xr:uid="{066D7A64-2A15-493A-89F9-E21854D10CBE}"/>
+    <hyperlink ref="K5" r:id="rId2" xr:uid="{927146F4-935B-4192-BDB1-9C8962EF4929}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId3"/>
@@ -986,64 +1013,64 @@
         <v>2</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="E1" s="14" t="s">
         <v>43</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
         <v>46</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>47</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>48</v>
-      </c>
-      <c r="D2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
         <v>51</v>
-      </c>
-      <c r="B3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
         <v>54</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>55</v>
-      </c>
-      <c r="C4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>